<commit_message>
small change in the plan
</commit_message>
<xml_diff>
--- a/monitoring/project-plan.xlsx
+++ b/monitoring/project-plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jashp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jashp\OneDrive\Documents\BFMC-repos\Brain\monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B56EC24-0C42-4EC1-A0C6-693162009693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239ED925-716B-4B1D-A3C2-0D1216F2A4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Traffic sign detection</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Checkpoint</t>
-  </si>
-  <si>
-    <t>Mid-term quality gate</t>
   </si>
   <si>
     <t>4th report</t>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>Christmas</t>
+  </si>
+  <si>
+    <t>Qualifications</t>
+  </si>
+  <si>
+    <t>5th report</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -795,6 +798,30 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -805,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -903,13 +930,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -940,16 +961,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -993,37 +1007,115 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1041,103 +1133,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1420,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA67"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="67" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF18" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1433,7 +1433,7 @@
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
@@ -1444,19 +1444,19 @@
     <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
     <col min="20" max="20" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8" customWidth="1"/>
     <col min="23" max="23" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.6640625" customWidth="1"/>
-    <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="26" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="2000" max="2000" width="2.33203125" customWidth="1"/>
+    <col min="25" max="27" width="8" customWidth="1"/>
+    <col min="28" max="28" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2002" max="2002" width="2.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="6">
         <f>B1+1</f>
@@ -1474,15 +1474,15 @@
         <f>D1+1</f>
         <v>3</v>
       </c>
-      <c r="F1" s="56">
+      <c r="F1" s="51">
         <f t="shared" ref="F1:Y1" si="0">E1+1</f>
         <v>4</v>
       </c>
-      <c r="G1" s="114">
+      <c r="G1" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" s="114">
+      <c r="H1" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1494,7 +1494,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K1" s="56">
+      <c r="K1" s="51">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -1510,7 +1510,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O1" s="56">
+      <c r="O1" s="51">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -1542,7 +1542,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="W1" s="56">
+      <c r="W1" s="51">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
@@ -1557,11 +1557,18 @@
       <c r="Z1" s="6">
         <v>24</v>
       </c>
-      <c r="AA1" s="7">
+      <c r="AA1" s="6">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB1" s="51">
+        <f t="shared" ref="AB1" si="1">AA1+1</f>
+        <v>26</v>
+      </c>
+      <c r="AC1" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1577,352 +1584,371 @@
         <f>D2+7</f>
         <v>45628</v>
       </c>
-      <c r="F2" s="57">
-        <f t="shared" ref="F2:O2" si="1">E2+7</f>
+      <c r="F2" s="52">
+        <f t="shared" ref="F2:O2" si="2">E2+7</f>
         <v>45635</v>
       </c>
-      <c r="G2" s="115">
-        <f t="shared" si="1"/>
+      <c r="G2" s="19">
+        <f t="shared" si="2"/>
         <v>45642</v>
       </c>
-      <c r="H2" s="115">
-        <f t="shared" si="1"/>
+      <c r="H2" s="19">
+        <f t="shared" si="2"/>
         <v>45649</v>
       </c>
       <c r="I2" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45656</v>
       </c>
       <c r="J2" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45663</v>
       </c>
-      <c r="K2" s="57">
-        <f t="shared" si="1"/>
+      <c r="K2" s="52">
+        <f t="shared" si="2"/>
         <v>45670</v>
       </c>
       <c r="L2" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45677</v>
       </c>
       <c r="M2" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45684</v>
       </c>
       <c r="N2" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45691</v>
       </c>
-      <c r="O2" s="57">
-        <f t="shared" si="1"/>
+      <c r="O2" s="52">
+        <f t="shared" si="2"/>
         <v>45698</v>
       </c>
       <c r="P2" s="19">
-        <f t="shared" ref="P2:AA2" si="2">O2+7</f>
+        <f t="shared" ref="P2:AC2" si="3">O2+7</f>
         <v>45705</v>
       </c>
       <c r="Q2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45712</v>
       </c>
       <c r="R2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45719</v>
       </c>
       <c r="S2" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45726</v>
       </c>
       <c r="T2" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45733</v>
       </c>
       <c r="U2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45740</v>
       </c>
       <c r="V2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45747</v>
       </c>
-      <c r="W2" s="57">
-        <f t="shared" si="2"/>
+      <c r="W2" s="52">
+        <f t="shared" si="3"/>
         <v>45754</v>
       </c>
       <c r="X2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45761</v>
       </c>
       <c r="Y2" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45768</v>
       </c>
       <c r="Z2" s="19">
-        <f t="shared" si="2"/>
+        <f>Y2+7</f>
         <v>45775</v>
       </c>
-      <c r="AA2" s="8">
-        <f t="shared" si="2"/>
+      <c r="AA2" s="19">
+        <f>Z2+7</f>
         <v>45782</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="93" t="s">
+      <c r="AB2" s="52">
+        <f t="shared" si="3"/>
+        <v>45789</v>
+      </c>
+      <c r="AC2" s="8">
+        <f t="shared" si="3"/>
+        <v>45796</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="D3" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="90"/>
       <c r="T3" s="31"/>
       <c r="U3" s="31"/>
       <c r="V3" s="31"/>
-      <c r="W3" s="69"/>
+      <c r="W3" s="64"/>
       <c r="X3" s="38"/>
       <c r="Y3" s="38"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="108" t="s">
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="70" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="40"/>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="88"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="95"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
       <c r="T4" s="37"/>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
-      <c r="W4" s="58"/>
+      <c r="W4" s="53"/>
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="109"/>
-    </row>
-    <row r="5" spans="1:27" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="40"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="53"/>
+      <c r="AC4" s="71"/>
+    </row>
+    <row r="5" spans="1:29" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="88"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="113"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="72"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
       <c r="S5" s="21"/>
-      <c r="T5" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="79"/>
-      <c r="V5" s="79"/>
-      <c r="W5" s="79"/>
-      <c r="X5" s="80" t="s">
+      <c r="T5" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="81"/>
-      <c r="AA5" s="109"/>
-    </row>
-    <row r="6" spans="1:27" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="76" t="s">
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y5" s="77"/>
+      <c r="Z5" s="110"/>
+      <c r="AA5" s="110"/>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="71"/>
+    </row>
+    <row r="6" spans="1:29" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="78"/>
-      <c r="I6" s="101" t="s">
+      <c r="E6" s="98"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="99"/>
+      <c r="I6" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="77"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="85" t="s">
+      <c r="J6" s="98"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="90" t="s">
+      <c r="M6" s="107"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="108"/>
+      <c r="P6" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
       <c r="T6" s="31"/>
       <c r="U6" s="31"/>
       <c r="V6" s="31"/>
-      <c r="W6" s="70"/>
+      <c r="W6" s="65"/>
       <c r="X6" s="32"/>
       <c r="Y6" s="32"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="109"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="94"/>
-      <c r="C7" s="74"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="71"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="94"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="88"/>
       <c r="D7" s="34"/>
       <c r="E7" s="25"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="117"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="59"/>
+      <c r="K7" s="54"/>
       <c r="L7" s="25"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="88" t="s">
+      <c r="N7" s="109" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
-      <c r="S7" s="88"/>
-      <c r="T7" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
       <c r="X7" s="30"/>
       <c r="Y7" s="30"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="109"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="99"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="74"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="71"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" s="95"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="34"/>
       <c r="E8" s="25"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="117"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="59"/>
+      <c r="K8" s="54"/>
       <c r="L8" s="25"/>
       <c r="M8" s="25"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="83" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q8" s="83"/>
-      <c r="R8" s="83"/>
-      <c r="S8" s="83"/>
-      <c r="T8" s="83" t="s">
+      <c r="O8" s="60"/>
+      <c r="P8" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="86"/>
+      <c r="T8" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="U8" s="83"/>
-      <c r="V8" s="83"/>
-      <c r="W8" s="83"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
       <c r="X8" s="30"/>
       <c r="Y8" s="30"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="109"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="74"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="71"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="95"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="34"/>
       <c r="E9" s="25"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="116"/>
-      <c r="H9" s="117"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="25"/>
       <c r="I9" s="25"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="59"/>
+      <c r="K9" s="54"/>
       <c r="L9" s="25"/>
       <c r="M9" s="25"/>
       <c r="N9" s="28"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="89" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="89"/>
-      <c r="S9" s="89"/>
-      <c r="T9" s="89"/>
-      <c r="U9" s="89"/>
-      <c r="V9" s="89"/>
-      <c r="W9" s="89"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
+      <c r="U9" s="73"/>
+      <c r="V9" s="73"/>
+      <c r="W9" s="73"/>
       <c r="X9" s="30"/>
       <c r="Y9" s="30"/>
-      <c r="Z9" s="35"/>
-      <c r="AA9" s="109"/>
-    </row>
-    <row r="10" spans="1:27" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="42"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="71"/>
+    </row>
+    <row r="10" spans="1:29" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="96"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="65"/>
+      <c r="K10" s="60"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="59"/>
+      <c r="O10" s="54"/>
       <c r="P10" s="25"/>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
@@ -1930,405 +1956,429 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y10" s="80"/>
-      <c r="Z10" s="81"/>
-      <c r="AA10" s="109"/>
-    </row>
-    <row r="11" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="103" t="s">
+      <c r="W10" s="62"/>
+      <c r="X10" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y10" s="77"/>
+      <c r="Z10" s="110"/>
+      <c r="AA10" s="110"/>
+      <c r="AB10" s="78"/>
+      <c r="AC10" s="71"/>
+    </row>
+    <row r="11" spans="1:29" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="75"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="104"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="104"/>
-      <c r="K11" s="104"/>
-      <c r="L11" s="104" t="s">
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="104"/>
-      <c r="N11" s="104"/>
-      <c r="O11" s="104"/>
-      <c r="P11" s="105" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="105"/>
+      <c r="Q11" s="87"/>
+      <c r="R11" s="87"/>
+      <c r="S11" s="87"/>
       <c r="T11" s="32"/>
       <c r="U11" s="32"/>
       <c r="V11" s="32"/>
       <c r="W11" s="32"/>
-      <c r="X11" s="51"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="109"/>
-    </row>
-    <row r="12" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="42"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="71"/>
+    </row>
+    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="88"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="83"/>
-      <c r="N12" s="83"/>
-      <c r="O12" s="83"/>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
-      <c r="R12" s="83"/>
-      <c r="S12" s="83"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="86" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
       <c r="V12" s="25"/>
       <c r="W12" s="25"/>
       <c r="X12" s="28"/>
       <c r="Y12" s="28"/>
-      <c r="Z12" s="53"/>
-      <c r="AA12" s="109"/>
-    </row>
-    <row r="13" spans="1:27" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="74"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="42"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="71"/>
+    </row>
+    <row r="13" spans="1:29" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="88"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="65"/>
+      <c r="K13" s="60"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="65"/>
+      <c r="O13" s="60"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
       <c r="R13" s="30"/>
       <c r="S13" s="29"/>
-      <c r="T13" s="79" t="s">
+      <c r="T13" s="83" t="s">
+        <v>37</v>
+      </c>
+      <c r="U13" s="83"/>
+      <c r="V13" s="83"/>
+      <c r="W13" s="83"/>
+      <c r="X13" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y13" s="77"/>
+      <c r="Z13" s="110"/>
+      <c r="AA13" s="110"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="71"/>
+    </row>
+    <row r="14" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="U13" s="79"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="79"/>
-      <c r="X13" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y13" s="80"/>
-      <c r="Z13" s="81"/>
-      <c r="AA13" s="109"/>
-    </row>
-    <row r="14" spans="1:27" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="96" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="103" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="90" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="104" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="U14" s="112"/>
-      <c r="V14" s="112"/>
-      <c r="W14" s="112"/>
+      <c r="U14" s="80"/>
+      <c r="V14" s="80"/>
+      <c r="W14" s="80"/>
       <c r="X14" s="32"/>
       <c r="Y14" s="32"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="109"/>
-    </row>
-    <row r="15" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="97"/>
-      <c r="B15" s="94"/>
-      <c r="C15" s="75"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="71"/>
+    </row>
+    <row r="15" spans="1:29" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="93"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="23"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="117"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="61"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="30"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="56"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-      <c r="O15" s="65"/>
+      <c r="O15" s="60"/>
       <c r="Q15" s="30"/>
       <c r="R15" s="30"/>
       <c r="S15" s="29"/>
-      <c r="T15" s="43"/>
+      <c r="T15" s="41"/>
       <c r="U15" s="30"/>
       <c r="V15" s="30"/>
-      <c r="W15" s="67"/>
-      <c r="X15" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y15" s="80"/>
-      <c r="Z15" s="81"/>
-      <c r="AA15" s="109"/>
-    </row>
-    <row r="16" spans="1:27" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="93" t="s">
+      <c r="W15" s="62"/>
+      <c r="X15" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y15" s="77"/>
+      <c r="Z15" s="110"/>
+      <c r="AA15" s="110"/>
+      <c r="AB15" s="78"/>
+      <c r="AC15" s="71"/>
+    </row>
+    <row r="16" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="76" t="s">
+      <c r="B16" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="77"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="104" t="s">
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="99"/>
+      <c r="L16" s="79" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="79"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="112" t="s">
-        <v>42</v>
-      </c>
-      <c r="U16" s="112"/>
-      <c r="V16" s="112"/>
-      <c r="W16" s="112"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="80"/>
+      <c r="W16" s="80"/>
       <c r="X16" s="32"/>
       <c r="Y16" s="32"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="109"/>
-    </row>
-    <row r="17" spans="1:27" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="82" t="s">
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="71"/>
+    </row>
+    <row r="17" spans="1:29" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
-      <c r="H17" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="89"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="65"/>
+      <c r="O17" s="60"/>
       <c r="S17" s="29"/>
-      <c r="T17" s="43"/>
+      <c r="T17" s="41"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
-      <c r="W17" s="67"/>
-      <c r="Z17" s="55"/>
-      <c r="AA17" s="109"/>
-    </row>
-    <row r="18" spans="1:27" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="94"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="82" t="s">
+      <c r="W17" s="62"/>
+      <c r="AB17" s="62"/>
+      <c r="AC17" s="71"/>
+    </row>
+    <row r="18" spans="1:29" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="118"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="30"/>
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="84"/>
-      <c r="N18" s="84"/>
-      <c r="O18" s="67"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="105"/>
+      <c r="N18" s="105"/>
+      <c r="O18" s="62"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="30"/>
       <c r="R18" s="30"/>
       <c r="S18" s="29"/>
-      <c r="T18" s="43"/>
+      <c r="T18" s="41"/>
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
-      <c r="W18" s="67"/>
-      <c r="Z18" s="55"/>
-      <c r="AA18" s="109"/>
-    </row>
-    <row r="19" spans="1:27" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="111"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="75"/>
+      <c r="W18" s="62"/>
+      <c r="AB18" s="62"/>
+      <c r="AC18" s="71"/>
+    </row>
+    <row r="19" spans="1:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="24"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="119"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
       <c r="S19" s="36"/>
-      <c r="T19" s="50"/>
-      <c r="U19" s="49"/>
-      <c r="V19" s="49"/>
-      <c r="W19" s="68"/>
-      <c r="X19" s="106" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y19" s="106"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="110"/>
-    </row>
-    <row r="20" spans="1:27" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T19" s="48"/>
+      <c r="U19" s="47"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="63"/>
+      <c r="X19" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y19" s="68"/>
+      <c r="Z19" s="111"/>
+      <c r="AA19" s="111"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="72"/>
+    </row>
+    <row r="20" spans="1:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="63">
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="58">
         <f>F2+6</f>
         <v>45641</v>
       </c>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="63">
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="58">
         <f>K2+6</f>
         <v>45676</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
       <c r="N20" s="26"/>
-      <c r="O20" s="63">
+      <c r="O20" s="58">
         <f>O2+6</f>
         <v>45704</v>
       </c>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
       <c r="S20" s="14">
         <f>S2+6</f>
         <v>45732</v>
       </c>
-      <c r="T20" s="50"/>
-      <c r="U20" s="49"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="47"/>
       <c r="V20" s="26"/>
-      <c r="W20" s="63">
+      <c r="W20" s="58">
         <f>W2+6</f>
         <v>45760</v>
       </c>
-      <c r="X20" s="49"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="49"/>
-      <c r="AA20" s="15">
-        <f>AA2+6</f>
-        <v>45788</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X20" s="47"/>
+      <c r="Y20" s="47"/>
+      <c r="Z20" s="47"/>
+      <c r="AA20" s="47"/>
+      <c r="AB20" s="58">
+        <f>AB2+6</f>
+        <v>45795</v>
+      </c>
+      <c r="AC20" s="15">
+        <f>AC2+6</f>
+        <v>45802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="122" t="s">
+      <c r="E21" s="42"/>
+      <c r="F21" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="84"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="122"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="17" t="s">
+      <c r="T21" s="44"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="43"/>
+      <c r="W21" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="T21" s="46"/>
-      <c r="U21" s="44"/>
-      <c r="V21" s="45"/>
-      <c r="W21" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="44"/>
-      <c r="Z21" s="44"/>
-      <c r="AA21" s="12" t="s">
+      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC21" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
@@ -2364,28 +2414,22 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="X19:Z19"/>
-    <mergeCell ref="AA3:AA19"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="L16:O16"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="T16:W16"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="D14:K14"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="L12:S12"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C3:C15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P9:W9"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="D3:J3"/>
@@ -2397,22 +2441,28 @@
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C3:C15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="P9:W9"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="L12:S12"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="X19:AB19"/>
+    <mergeCell ref="AC3:AC19"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="X15:AB15"/>
+    <mergeCell ref="L16:O16"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="T16:W16"/>
+    <mergeCell ref="X13:AB13"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="P6:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>